<commit_message>
Allocated Group use cases to myself
</commit_message>
<xml_diff>
--- a/schoolwork/UseCaseAllocation.xlsx
+++ b/schoolwork/UseCaseAllocation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ajrobinson/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jerls\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9541F881-30A1-3443-BAFA-2792079EB49D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{503866CD-D647-4E4C-A4C4-37E6F71B0D2C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="3400" windowWidth="28040" windowHeight="16300" xr2:uid="{39673AE3-FEE1-374E-86B3-EBA37C3D3889}"/>
+    <workbookView xWindow="120" yWindow="1740" windowWidth="13035" windowHeight="11385" xr2:uid="{39673AE3-FEE1-374E-86B3-EBA37C3D3889}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Member</t>
   </si>
@@ -78,6 +78,18 @@
   </si>
   <si>
     <t>DeleteMessage</t>
+  </si>
+  <si>
+    <t>CreateAccount</t>
+  </si>
+  <si>
+    <t>ViewMessage</t>
+  </si>
+  <si>
+    <t>CreateGroup</t>
+  </si>
+  <si>
+    <t>JoinGroup</t>
   </si>
 </sst>
 </file>
@@ -450,23 +462,23 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.6640625" customWidth="1"/>
-    <col min="2" max="2" width="20.83203125" customWidth="1"/>
+    <col min="1" max="1" width="17.625" customWidth="1"/>
+    <col min="2" max="2" width="20.875" customWidth="1"/>
     <col min="3" max="3" width="22" customWidth="1"/>
-    <col min="4" max="4" width="20.83203125" customWidth="1"/>
+    <col min="4" max="4" width="20.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -480,7 +492,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -491,22 +503,28 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -517,9 +535,15 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
+      </c>
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>